<commit_message>
create data_regression and split code from data compiling + all outputs
</commit_message>
<xml_diff>
--- a/Output_analysis/Linear_regression_all_indicators.xlsx
+++ b/Output_analysis/Linear_regression_all_indicators.xlsx
@@ -543,7 +543,7 @@
         <v>-0.1886755593162644</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00745901254805089</v>
+        <v>0.007459012548050867</v>
       </c>
       <c r="I3" t="n">
         <v>0.002503584901896897</v>
@@ -570,22 +570,22 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>-0.003046463603018163</v>
+        <v>-0.003046463603018164</v>
       </c>
       <c r="F4" t="n">
         <v>-1.736276138117242</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.1829645928627698</v>
+        <v>-0.1829645928627699</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01267403984881358</v>
+        <v>0.01267403984881357</v>
       </c>
       <c r="I4" t="n">
         <v>0.001210067807522428</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1829645928627698</v>
+        <v>0.1829645928627699</v>
       </c>
     </row>
     <row r="5">
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>-0.0005644824448269858</v>
+        <v>-0.0005644824448269857</v>
       </c>
       <c r="F5" t="n">
         <v>1.269568207576246</v>
@@ -615,7 +615,7 @@
         <v>-0.1671822158355729</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01917620139000204</v>
+        <v>0.01917620139000209</v>
       </c>
       <c r="I5" t="n">
         <v>0.0002390032596854748</v>
@@ -642,10 +642,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>-0.0006356249480340517</v>
+        <v>-0.0006356249480340518</v>
       </c>
       <c r="F6" t="n">
-        <v>1.209300279572703</v>
+        <v>1.209300279572704</v>
       </c>
       <c r="G6" t="n">
         <v>-0.1656338594377076</v>
@@ -690,7 +690,7 @@
         <v>0.02659036543293193</v>
       </c>
       <c r="I7" t="n">
-        <v>0.02457824563654961</v>
+        <v>0.02457824563654962</v>
       </c>
       <c r="J7" t="n">
         <v>0.1634873832211779</v>
@@ -723,7 +723,7 @@
         <v>0.1632333331831002</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0260040687857451</v>
+        <v>0.02600406878574506</v>
       </c>
       <c r="I8" t="n">
         <v>0.0009686738468537766</v>
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.002880524400756869</v>
+        <v>0.002880524400756868</v>
       </c>
       <c r="F9" t="n">
         <v>5.660941722369918</v>
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>-0.007927213345223998</v>
+        <v>-0.007927213345223994</v>
       </c>
       <c r="F12" t="n">
         <v>14.04324635353203</v>
@@ -867,7 +867,7 @@
         <v>-0.1295639626904165</v>
       </c>
       <c r="H12" t="n">
-        <v>0.06746838236269838</v>
+        <v>0.06746838236269843</v>
       </c>
       <c r="I12" t="n">
         <v>0.004311491902337861</v>
@@ -894,7 +894,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>-6180.995066092756</v>
+        <v>-6180.995066092755</v>
       </c>
       <c r="F13" t="n">
         <v>13208165.48638866</v>
@@ -903,7 +903,7 @@
         <v>-0.1294109839210498</v>
       </c>
       <c r="H13" t="n">
-        <v>0.08081213652822454</v>
+        <v>0.08081213652822457</v>
       </c>
       <c r="I13" t="n">
         <v>3520.307213847446</v>
@@ -1116,16 +1116,16 @@
         <v>12.15085256337629</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.09712786516027325</v>
+        <v>-0.09712786516027326</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1712423337795015</v>
+        <v>0.1712423337795014</v>
       </c>
       <c r="I19" t="n">
-        <v>0.00286238541201678</v>
+        <v>0.002862385412016779</v>
       </c>
       <c r="J19" t="n">
-        <v>0.09712786516027325</v>
+        <v>0.09712786516027326</v>
       </c>
     </row>
     <row r="20">
@@ -1146,22 +1146,22 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>-0.007988184214698562</v>
+        <v>-0.007988184214698565</v>
       </c>
       <c r="F20" t="n">
         <v>135.3739694905287</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.09509510052265459</v>
+        <v>-0.09509510052265463</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2346242359737183</v>
+        <v>0.2346242359737181</v>
       </c>
       <c r="I20" t="n">
         <v>0.006695068399413947</v>
       </c>
       <c r="J20" t="n">
-        <v>0.09509510052265459</v>
+        <v>0.09509510052265463</v>
       </c>
     </row>
     <row r="21">
@@ -1221,19 +1221,19 @@
         <v>0.001443076465579541</v>
       </c>
       <c r="F22" t="n">
-        <v>4.066577143110764</v>
+        <v>4.066577143110763</v>
       </c>
       <c r="G22" t="n">
-        <v>0.08762419010529818</v>
+        <v>0.08762419010529819</v>
       </c>
       <c r="H22" t="n">
-        <v>0.2219942334107639</v>
+        <v>0.2219942334107638</v>
       </c>
       <c r="I22" t="n">
         <v>0.001177852132107766</v>
       </c>
       <c r="J22" t="n">
-        <v>0.08762419010529818</v>
+        <v>0.08762419010529819</v>
       </c>
     </row>
     <row r="23">
@@ -1254,13 +1254,13 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.00622204871053424</v>
+        <v>0.006222048710534241</v>
       </c>
       <c r="F23" t="n">
         <v>36.53191839966643</v>
       </c>
       <c r="G23" t="n">
-        <v>0.08544189655521531</v>
+        <v>0.08544189655521532</v>
       </c>
       <c r="H23" t="n">
         <v>0.2254894153852886</v>
@@ -1269,7 +1269,7 @@
         <v>0.005117683687886346</v>
       </c>
       <c r="J23" t="n">
-        <v>0.08544189655521531</v>
+        <v>0.08544189655521532</v>
       </c>
     </row>
     <row r="24">
@@ -1332,16 +1332,16 @@
         <v>60.55617530788305</v>
       </c>
       <c r="G25" t="n">
-        <v>0.08236974468915065</v>
+        <v>0.08236974468915062</v>
       </c>
       <c r="H25" t="n">
-        <v>0.2426746541165328</v>
+        <v>0.2426746541165329</v>
       </c>
       <c r="I25" t="n">
         <v>0.009186000606424145</v>
       </c>
       <c r="J25" t="n">
-        <v>0.08236974468915065</v>
+        <v>0.08236974468915062</v>
       </c>
     </row>
     <row r="26">
@@ -1434,13 +1434,13 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>-0.0006733058260378087</v>
+        <v>-0.000673305826037809</v>
       </c>
       <c r="F28" t="n">
-        <v>6.062098833635806</v>
+        <v>6.062098833635807</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.0665447685104442</v>
+        <v>-0.06654476851044423</v>
       </c>
       <c r="H28" t="n">
         <v>0.3491575651582812</v>
@@ -1449,7 +1449,7 @@
         <v>0.00071746736364266</v>
       </c>
       <c r="J28" t="n">
-        <v>0.0665447685104442</v>
+        <v>0.06654476851044423</v>
       </c>
     </row>
     <row r="29">
@@ -1470,22 +1470,22 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>-0.0055256851384317</v>
+        <v>-0.005525685138431699</v>
       </c>
       <c r="F29" t="n">
         <v>17.21875411208789</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.06244928549859528</v>
+        <v>-0.06244928549859526</v>
       </c>
       <c r="H29" t="n">
-        <v>0.3882584969479823</v>
+        <v>0.3882584969479825</v>
       </c>
       <c r="I29" t="n">
         <v>0.006389891236958421</v>
       </c>
       <c r="J29" t="n">
-        <v>0.06244928549859528</v>
+        <v>0.06244928549859526</v>
       </c>
     </row>
     <row r="30">
@@ -1512,16 +1512,16 @@
         <v>10.97308527523539</v>
       </c>
       <c r="G30" t="n">
-        <v>0.05869751122167888</v>
+        <v>0.05869751122167886</v>
       </c>
       <c r="H30" t="n">
-        <v>0.4286706712263356</v>
+        <v>0.4286706712263358</v>
       </c>
       <c r="I30" t="n">
         <v>0.002944880208632211</v>
       </c>
       <c r="J30" t="n">
-        <v>0.05869751122167888</v>
+        <v>0.05869751122167886</v>
       </c>
     </row>
     <row r="31">
@@ -1542,22 +1542,22 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>-3.592897306428081</v>
+        <v>-3.592897306428078</v>
       </c>
       <c r="F31" t="n">
         <v>20735.98239013982</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.05779364360557142</v>
+        <v>-0.05779364360557138</v>
       </c>
       <c r="H31" t="n">
-        <v>0.4210456587177294</v>
+        <v>0.4210456587177295</v>
       </c>
       <c r="I31" t="n">
         <v>4.455919693129604</v>
       </c>
       <c r="J31" t="n">
-        <v>0.05779364360557142</v>
+        <v>0.05779364360557138</v>
       </c>
     </row>
     <row r="32">
@@ -1578,22 +1578,22 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.0004451896150952703</v>
+        <v>0.0004451896150952699</v>
       </c>
       <c r="F32" t="n">
         <v>7.603332949274667</v>
       </c>
       <c r="G32" t="n">
-        <v>0.05759532214712781</v>
+        <v>0.05759532214712778</v>
       </c>
       <c r="H32" t="n">
-        <v>0.4238451139263596</v>
+        <v>0.4238451139263597</v>
       </c>
       <c r="I32" t="n">
-        <v>0.000555466198222145</v>
+        <v>0.0005554661982221449</v>
       </c>
       <c r="J32" t="n">
-        <v>0.05759532214712781</v>
+        <v>0.05759532214712778</v>
       </c>
     </row>
     <row r="33">
@@ -1614,22 +1614,22 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.001926383135230008</v>
+        <v>0.00192638313523001</v>
       </c>
       <c r="F33" t="n">
-        <v>94.96848480887351</v>
+        <v>94.96848480887353</v>
       </c>
       <c r="G33" t="n">
-        <v>0.05726388473891442</v>
+        <v>0.05726388473891447</v>
       </c>
       <c r="H33" t="n">
-        <v>0.4595957685354668</v>
+        <v>0.4595957685354665</v>
       </c>
       <c r="I33" t="n">
-        <v>0.002598904948737208</v>
+        <v>0.002598904948737209</v>
       </c>
       <c r="J33" t="n">
-        <v>0.05726388473891442</v>
+        <v>0.05726388473891447</v>
       </c>
     </row>
     <row r="34">
@@ -1650,22 +1650,22 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>-0.0002187846718425098</v>
+        <v>-0.0002187846718425097</v>
       </c>
       <c r="F34" t="n">
         <v>2.465053769745219</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.05674458104962053</v>
+        <v>-0.0567445810496205</v>
       </c>
       <c r="H34" t="n">
-        <v>0.4271654134110636</v>
+        <v>0.4271654134110638</v>
       </c>
       <c r="I34" t="n">
         <v>0.000274956588958861</v>
       </c>
       <c r="J34" t="n">
-        <v>0.05674458104962053</v>
+        <v>0.0567445810496205</v>
       </c>
     </row>
     <row r="35">
@@ -1686,22 +1686,22 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>-0.000599674130503996</v>
+        <v>-0.0005996741305039964</v>
       </c>
       <c r="F35" t="n">
         <v>4.494898180659098</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.05414319306008925</v>
+        <v>-0.05414319306008929</v>
       </c>
       <c r="H35" t="n">
-        <v>0.4557408656297243</v>
+        <v>0.4557408656297238</v>
       </c>
       <c r="I35" t="n">
-        <v>0.0008023376098333617</v>
+        <v>0.0008023376098333618</v>
       </c>
       <c r="J35" t="n">
-        <v>0.05414319306008925</v>
+        <v>0.05414319306008929</v>
       </c>
     </row>
     <row r="36">
@@ -1764,16 +1764,16 @@
         <v>13.31389319740318</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.03691311405371973</v>
+        <v>-0.03691311405371975</v>
       </c>
       <c r="H37" t="n">
-        <v>0.6169310724136428</v>
+        <v>0.6169310724136426</v>
       </c>
       <c r="I37" t="n">
         <v>0.002629557037709445</v>
       </c>
       <c r="J37" t="n">
-        <v>0.03691311405371973</v>
+        <v>0.03691311405371975</v>
       </c>
     </row>
     <row r="38">
@@ -1794,22 +1794,22 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.0004538459132602376</v>
+        <v>0.0004538459132602374</v>
       </c>
       <c r="F38" t="n">
         <v>4.706120378434015</v>
       </c>
       <c r="G38" t="n">
-        <v>0.03491427558271145</v>
+        <v>0.03491427558271144</v>
       </c>
       <c r="H38" t="n">
-        <v>0.6209313371490713</v>
+        <v>0.6209313371490714</v>
       </c>
       <c r="I38" t="n">
         <v>0.0009163101546164911</v>
       </c>
       <c r="J38" t="n">
-        <v>0.03491427558271145</v>
+        <v>0.03491427558271144</v>
       </c>
     </row>
     <row r="39">
@@ -1830,22 +1830,22 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.0002370484446392983</v>
+        <v>0.0002370484446392985</v>
       </c>
       <c r="F39" t="n">
         <v>2.011810125540316</v>
       </c>
       <c r="G39" t="n">
-        <v>0.027728072141536</v>
+        <v>0.02772807214153601</v>
       </c>
       <c r="H39" t="n">
-        <v>0.7056347441916659</v>
+        <v>0.7056347441916657</v>
       </c>
       <c r="I39" t="n">
         <v>0.0006266051293925474</v>
       </c>
       <c r="J39" t="n">
-        <v>0.027728072141536</v>
+        <v>0.02772807214153601</v>
       </c>
     </row>
     <row r="40">
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>7.659509341017447e-05</v>
+        <v>7.659509341017445e-05</v>
       </c>
       <c r="F41" t="n">
         <v>3.631046676330005</v>
@@ -1938,7 +1938,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>-0.3950842969408914</v>
+        <v>-0.3950842969408912</v>
       </c>
       <c r="F42" t="n">
         <v>9464.241937993702</v>
@@ -1974,13 +1974,13 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>-0.0008657000696049978</v>
+        <v>-0.0008657000696049984</v>
       </c>
       <c r="F43" t="n">
         <v>36.76706681384611</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.01195520763335026</v>
+        <v>-0.01195520763335027</v>
       </c>
       <c r="H43" t="n">
         <v>0.8655687843302234</v>
@@ -1989,7 +1989,7 @@
         <v>0.00510718114676217</v>
       </c>
       <c r="J43" t="n">
-        <v>0.01195520763335026</v>
+        <v>0.01195520763335027</v>
       </c>
     </row>
     <row r="44">
@@ -2010,22 +2010,22 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.0003710550454216065</v>
+        <v>0.0003710550454216064</v>
       </c>
       <c r="F44" t="n">
         <v>13.01523819056615</v>
       </c>
       <c r="G44" t="n">
-        <v>0.007353595734597772</v>
+        <v>0.00735359573459777</v>
       </c>
       <c r="H44" t="n">
-        <v>0.9221733224233754</v>
+        <v>0.9221733224233755</v>
       </c>
       <c r="I44" t="n">
         <v>0.00379262771791512</v>
       </c>
       <c r="J44" t="n">
-        <v>0.007353595734597772</v>
+        <v>0.00735359573459777</v>
       </c>
     </row>
     <row r="45">
@@ -2046,22 +2046,22 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>-0.0001710091435240589</v>
+        <v>-0.0001710091435240585</v>
       </c>
       <c r="F45" t="n">
         <v>7.474280954536821</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.005777349714305521</v>
+        <v>-0.005777349714305506</v>
       </c>
       <c r="H45" t="n">
-        <v>0.936277177461892</v>
+        <v>0.9362771774618922</v>
       </c>
       <c r="I45" t="n">
         <v>0.002136155248214013</v>
       </c>
       <c r="J45" t="n">
-        <v>0.005777349714305521</v>
+        <v>0.005777349714305506</v>
       </c>
     </row>
     <row r="46">
@@ -2082,13 +2082,13 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>7.718782663024841e-05</v>
+        <v>7.71878266302484e-05</v>
       </c>
       <c r="F46" t="n">
         <v>5.825472247196402</v>
       </c>
       <c r="G46" t="n">
-        <v>0.005454733543747017</v>
+        <v>0.005454733543747016</v>
       </c>
       <c r="H46" t="n">
         <v>0.9396720591605254</v>
@@ -2097,7 +2097,7 @@
         <v>0.001018568301059904</v>
       </c>
       <c r="J46" t="n">
-        <v>0.005454733543747017</v>
+        <v>0.005454733543747016</v>
       </c>
     </row>
     <row r="47">
@@ -2118,22 +2118,22 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.0001039112370298824</v>
+        <v>0.0001039112370298823</v>
       </c>
       <c r="F47" t="n">
         <v>72.2187594266311</v>
       </c>
       <c r="G47" t="n">
-        <v>0.004339335300323433</v>
+        <v>0.004339335300323431</v>
       </c>
       <c r="H47" t="n">
-        <v>0.9517429461362751</v>
+        <v>0.9517429461362752</v>
       </c>
       <c r="I47" t="n">
         <v>0.001714817516447844</v>
       </c>
       <c r="J47" t="n">
-        <v>0.004339335300323433</v>
+        <v>0.004339335300323431</v>
       </c>
     </row>
     <row r="48">
@@ -2154,22 +2154,22 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>-0.07263754893159202</v>
+        <v>-0.07263754893159231</v>
       </c>
       <c r="F48" t="n">
-        <v>7533.698790940319</v>
+        <v>7533.698790940317</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.002779807974725857</v>
+        <v>-0.002779807974725869</v>
       </c>
       <c r="H48" t="n">
-        <v>0.9706237073566406</v>
+        <v>0.9706237073566404</v>
       </c>
       <c r="I48" t="n">
         <v>1.969646880812565</v>
       </c>
       <c r="J48" t="n">
-        <v>0.002779807974725857</v>
+        <v>0.002779807974725869</v>
       </c>
     </row>
     <row r="49">
@@ -2190,22 +2190,22 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>-4.310117453905327e-05</v>
+        <v>-4.310117453905336e-05</v>
       </c>
       <c r="F49" t="n">
         <v>5.691321934339411</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.002671099504097558</v>
+        <v>-0.002671099504097563</v>
       </c>
       <c r="H49" t="n">
-        <v>0.9705139129012279</v>
+        <v>0.9705139129012278</v>
       </c>
       <c r="I49" t="n">
         <v>0.001164519793798672</v>
       </c>
       <c r="J49" t="n">
-        <v>0.002671099504097558</v>
+        <v>0.002671099504097563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>